<commit_message>
testing ime crep model
</commit_message>
<xml_diff>
--- a/data/crep_oceanographic/Gove2013_pone.0061974.s005.xlsx
+++ b/data/crep_oceanographic/Gove2013_pone.0061974.s005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrobinson/Documents/git-repos/PelagicReefs/data/crep_oceanographic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD2EC05-53A4-CE4E-A016-CBB29D255E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755AFBD5-8771-EE43-BB37-8087C6AC5801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="191">
   <si>
     <t>Sea Surface Temperature (°C)</t>
   </si>
@@ -527,16 +527,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Pearl &amp; Hermes Reef</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="9"/>
         <rFont val="Times New Roman"/>
@@ -1348,15 +1338,6 @@
       </rPr>
       <t>AGR</t>
     </r>
-  </si>
-  <si>
-    <t>reef_area_km2</t>
-  </si>
-  <si>
-    <t>atoll_island</t>
-  </si>
-  <si>
-    <t>Atoll</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1491,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1612,17 +1593,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1636,7 +1606,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
@@ -1653,42 +1623,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1745,26 +1679,47 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2081,7 +2036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="C3" sqref="A1:AO43"/>
     </sheetView>
   </sheetViews>
@@ -2112,50 +2067,50 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="11" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="17" t="s">
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="8" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="10"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="30"/>
     </row>
     <row r="2" spans="1:41" ht="37.25" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -7421,15 +7376,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W42"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="64">
+    <row r="1" spans="1:21" ht="64">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -7457,14 +7412,8 @@
       <c r="I1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -7492,23 +7441,17 @@
       <c r="I2" s="7">
         <v>39.265282173816402</v>
       </c>
-      <c r="J2" s="31">
-        <v>83.15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>194</v>
-      </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="23"/>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -7536,23 +7479,17 @@
       <c r="I3" s="7">
         <v>39.367662591687001</v>
       </c>
-      <c r="J3" s="31">
-        <v>101.52</v>
-      </c>
-      <c r="K3" t="s">
-        <v>194</v>
-      </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="26"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="M3" s="12"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="14"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -7580,23 +7517,17 @@
       <c r="I4" s="7">
         <v>39.666391361043203</v>
       </c>
-      <c r="J4" s="43">
-        <v>467.27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>194</v>
-      </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="30"/>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="18"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -7624,23 +7555,17 @@
       <c r="I5" s="7">
         <v>41.316668629743802</v>
       </c>
-      <c r="J5" s="31">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="K5" t="s">
-        <v>194</v>
-      </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="30"/>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="M5" s="16"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="18"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -7668,23 +7593,17 @@
       <c r="I6" s="7">
         <v>41.458515688671604</v>
       </c>
-      <c r="J6" s="31">
-        <v>488.13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="30"/>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="M6" s="16"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="18"/>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -7712,23 +7631,17 @@
       <c r="I7" s="7">
         <v>41.869655791977799</v>
       </c>
-      <c r="J7" s="31">
-        <v>3.03</v>
-      </c>
-      <c r="K7" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" s="39"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="41"/>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="M7" s="16"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="18"/>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -7756,23 +7669,17 @@
       <c r="I8" s="7">
         <v>43.398087518337398</v>
       </c>
-      <c r="J8" s="31">
-        <v>677.96</v>
-      </c>
-      <c r="K8" t="s">
-        <v>194</v>
-      </c>
-      <c r="O8" s="28"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="30"/>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="M8" s="16"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="18"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -7800,23 +7707,17 @@
       <c r="I9" s="7">
         <v>43.507914251705103</v>
       </c>
-      <c r="J9" s="31">
-        <v>1028.32</v>
-      </c>
-      <c r="K9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="30"/>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="M9" s="16"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="18"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -7844,21 +7745,17 @@
       <c r="I10" s="7">
         <v>43.638761033007299</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="30"/>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="M10" s="16"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="18"/>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -7886,23 +7783,17 @@
       <c r="I11" s="7">
         <v>43.007571252871003</v>
       </c>
-      <c r="J11" s="31">
-        <v>241.7</v>
-      </c>
-      <c r="K11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="28"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="30"/>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="18"/>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -7930,23 +7821,17 @@
       <c r="I12" s="7">
         <v>43.776517578175302</v>
       </c>
-      <c r="J12" s="31">
-        <v>108.06</v>
-      </c>
-      <c r="K12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="28"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="30"/>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="M12" s="16"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="18"/>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -7974,23 +7859,17 @@
       <c r="I13" s="7">
         <v>43.257167879286598</v>
       </c>
-      <c r="J13" s="31">
-        <v>422.72</v>
-      </c>
-      <c r="K13" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="30"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="M13" s="16"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="18"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -8018,23 +7897,17 @@
       <c r="I14" s="7">
         <v>44.381059030154901</v>
       </c>
-      <c r="J14" s="31">
-        <v>450.84</v>
-      </c>
-      <c r="K14" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" s="28"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="30"/>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="M14" s="16"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="18"/>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -8062,23 +7935,17 @@
       <c r="I15" s="7">
         <v>44.953106292626501</v>
       </c>
-      <c r="J15" s="31">
-        <v>450.84</v>
-      </c>
-      <c r="K15" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="28"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="30"/>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="M15" s="16"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="18"/>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -8106,23 +7973,17 @@
       <c r="I16" s="7">
         <v>43.7165007579462</v>
       </c>
-      <c r="J16" s="31">
-        <v>450.84</v>
-      </c>
-      <c r="K16" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="28"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="30"/>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="M16" s="16"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="18"/>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -8150,23 +8011,17 @@
       <c r="I17" s="7">
         <v>41.461423233859399</v>
       </c>
-      <c r="J17" s="31">
-        <v>201.67</v>
-      </c>
-      <c r="K17" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="28"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="30"/>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="M17" s="16"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="18"/>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
@@ -8194,23 +8049,17 @@
       <c r="I18" s="7">
         <v>45.552707998602898</v>
       </c>
-      <c r="J18" s="31">
-        <v>194.01</v>
-      </c>
-      <c r="K18" t="s">
-        <v>194</v>
-      </c>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="30"/>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="M18" s="16"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="18"/>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
@@ -8238,23 +8087,17 @@
       <c r="I19" s="7">
         <v>44.713863868513997</v>
       </c>
-      <c r="J19" s="37">
-        <v>19.18</v>
-      </c>
-      <c r="K19" t="s">
-        <v>194</v>
-      </c>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="30"/>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="M19" s="16"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="18"/>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
@@ -8282,23 +8125,17 @@
       <c r="I20" s="7">
         <v>43.201211776691103</v>
       </c>
-      <c r="J20" s="31">
-        <v>1.38</v>
-      </c>
-      <c r="K20" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="28"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="30"/>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="M20" s="16"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="18"/>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -8326,23 +8163,17 @@
       <c r="I21" s="7">
         <v>43.478261450692798</v>
       </c>
-      <c r="J21" s="31">
-        <v>3.17</v>
-      </c>
-      <c r="K21" t="s">
-        <v>3</v>
-      </c>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="30"/>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="M21" s="16"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="18"/>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -8370,23 +8201,17 @@
       <c r="I22" s="7">
         <v>43.121240790545997</v>
       </c>
-      <c r="J22" s="31">
-        <v>2.54</v>
-      </c>
-      <c r="K22" t="s">
-        <v>3</v>
-      </c>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="30"/>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="M22" s="16"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="18"/>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
@@ -8414,23 +8239,17 @@
       <c r="I23" s="7">
         <v>42.805033604998698</v>
       </c>
-      <c r="J23" s="43">
-        <v>9.5</v>
-      </c>
-      <c r="K23" t="s">
-        <v>3</v>
-      </c>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="30"/>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="M23" s="16"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="18"/>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
@@ -8458,23 +8277,17 @@
       <c r="I24" s="7">
         <v>43.1460346916598</v>
       </c>
-      <c r="J24" s="31">
-        <v>16.29</v>
-      </c>
-      <c r="K24" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="30"/>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="M24" s="16"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="18"/>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" s="5" t="s">
         <v>54</v>
       </c>
@@ -8502,23 +8315,17 @@
       <c r="I25" s="7">
         <v>43.4626099633252</v>
       </c>
-      <c r="J25" s="31">
-        <v>4.28</v>
-      </c>
-      <c r="K25" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="31"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="30"/>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="M25" s="16"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="18"/>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" s="5" t="s">
         <v>56</v>
       </c>
@@ -8546,23 +8353,17 @@
       <c r="I26" s="7">
         <v>43.663095668878803</v>
       </c>
-      <c r="J26" s="31">
-        <v>2</v>
-      </c>
-      <c r="K26" t="s">
-        <v>3</v>
-      </c>
-      <c r="O26" s="28"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="30"/>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="M26" s="16"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="18"/>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
@@ -8590,23 +8391,17 @@
       <c r="I27" s="7">
         <v>43.159807775061097</v>
       </c>
-      <c r="J27" s="31">
-        <v>2</v>
-      </c>
-      <c r="K27" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="28"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="32"/>
-      <c r="W27" s="30"/>
-    </row>
-    <row r="28" spans="1:23">
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="18"/>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -8634,23 +8429,17 @@
       <c r="I28" s="7">
         <v>43.310200750960497</v>
       </c>
-      <c r="J28" s="31">
-        <v>95.15</v>
-      </c>
-      <c r="K28" t="s">
-        <v>3</v>
-      </c>
-      <c r="O28" s="28"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="30"/>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="M28" s="16"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="18"/>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" s="5" t="s">
         <v>62</v>
       </c>
@@ -8678,23 +8467,17 @@
       <c r="I29" s="7">
         <v>42.806615452322802</v>
       </c>
-      <c r="J29" s="31">
-        <v>95.15</v>
-      </c>
-      <c r="K29" t="s">
-        <v>3</v>
-      </c>
-      <c r="O29" s="28"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="31"/>
-      <c r="U29" s="31"/>
-      <c r="V29" s="31"/>
-      <c r="W29" s="30"/>
-    </row>
-    <row r="30" spans="1:23">
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="18"/>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="5" t="s">
         <v>64</v>
       </c>
@@ -8722,23 +8505,17 @@
       <c r="I30" s="7">
         <v>43.5751960181627</v>
       </c>
-      <c r="J30" s="31">
-        <v>95.15</v>
-      </c>
-      <c r="K30" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="39"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="41"/>
-    </row>
-    <row r="31" spans="1:23">
+      <c r="M30" s="16"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="18"/>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" s="5" t="s">
         <v>66</v>
       </c>
@@ -8766,23 +8543,17 @@
       <c r="I31" s="7">
         <v>43.658483863080697</v>
       </c>
-      <c r="J31" s="31">
-        <v>16.03</v>
-      </c>
-      <c r="K31" t="s">
-        <v>3</v>
-      </c>
-      <c r="O31" s="28"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="31"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="31"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="30"/>
-    </row>
-    <row r="32" spans="1:23">
+      <c r="M31" s="16"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="18"/>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="5" t="s">
         <v>68</v>
       </c>
@@ -8810,23 +8581,17 @@
       <c r="I32" s="7">
         <v>42.636856768993901</v>
       </c>
-      <c r="J32" s="31">
-        <v>94.85</v>
-      </c>
-      <c r="K32" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="28"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="31"/>
-      <c r="U32" s="31"/>
-      <c r="V32" s="31"/>
-      <c r="W32" s="30"/>
-    </row>
-    <row r="33" spans="1:23">
+      <c r="M32" s="16"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="18"/>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" s="5" t="s">
         <v>70</v>
       </c>
@@ -8854,23 +8619,17 @@
       <c r="I33" s="7">
         <v>39.053144682151597</v>
       </c>
-      <c r="J33" s="31">
-        <v>47.63</v>
-      </c>
-      <c r="K33" t="s">
-        <v>194</v>
-      </c>
-      <c r="O33" s="28"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="31"/>
-      <c r="U33" s="31"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="30"/>
-    </row>
-    <row r="34" spans="1:23">
+      <c r="M33" s="16"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="18"/>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="5" t="s">
         <v>73</v>
       </c>
@@ -8898,23 +8657,17 @@
       <c r="I34" s="7">
         <v>39.209256130251198</v>
       </c>
-      <c r="J34" s="31">
-        <v>52.5</v>
-      </c>
-      <c r="K34" t="s">
-        <v>194</v>
-      </c>
-      <c r="O34" s="28"/>
-      <c r="P34" s="29"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="31"/>
-      <c r="U34" s="31"/>
-      <c r="V34" s="31"/>
-      <c r="W34" s="30"/>
-    </row>
-    <row r="35" spans="1:23">
+      <c r="M34" s="16"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="18"/>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="5" t="s">
         <v>75</v>
       </c>
@@ -8942,23 +8695,17 @@
       <c r="I35" s="7">
         <v>47.822408410758001</v>
       </c>
-      <c r="J35" s="31">
-        <v>2.57</v>
-      </c>
-      <c r="K35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" s="28"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="31"/>
-      <c r="T35" s="31"/>
-      <c r="U35" s="31"/>
-      <c r="V35" s="31"/>
-      <c r="W35" s="30"/>
-    </row>
-    <row r="36" spans="1:23">
+      <c r="M35" s="16"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="18"/>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="5" t="s">
         <v>77</v>
       </c>
@@ -8986,23 +8733,17 @@
       <c r="I36" s="7">
         <v>48.404574938875299</v>
       </c>
-      <c r="J36" s="31">
-        <v>4.43</v>
-      </c>
-      <c r="K36" t="s">
-        <v>194</v>
-      </c>
-      <c r="O36" s="28"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="31"/>
-      <c r="T36" s="31"/>
-      <c r="U36" s="31"/>
-      <c r="V36" s="31"/>
-      <c r="W36" s="30"/>
-    </row>
-    <row r="37" spans="1:23">
+      <c r="M36" s="16"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="18"/>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" s="5" t="s">
         <v>79</v>
       </c>
@@ -9030,23 +8771,17 @@
       <c r="I37" s="7">
         <v>50.188835268948601</v>
       </c>
-      <c r="J37" s="31">
-        <v>4.32</v>
-      </c>
-      <c r="K37" t="s">
-        <v>194</v>
-      </c>
-      <c r="O37" s="35"/>
-      <c r="P37" s="42"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="37"/>
-      <c r="U37" s="37"/>
-      <c r="V37" s="44"/>
-      <c r="W37" s="36"/>
-    </row>
-    <row r="38" spans="1:23">
+      <c r="M37" s="23"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="25"/>
+      <c r="S37" s="25"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="24"/>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" s="5" t="s">
         <v>81</v>
       </c>
@@ -9074,14 +8809,8 @@
       <c r="I38" s="7">
         <v>42.364848125509397</v>
       </c>
-      <c r="J38" s="31">
-        <v>2.82</v>
-      </c>
-      <c r="K38" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23">
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" s="5" t="s">
         <v>84</v>
       </c>
@@ -9109,14 +8838,8 @@
       <c r="I39" s="7">
         <v>41.763511624805503</v>
       </c>
-      <c r="J39" s="27">
-        <v>22.42</v>
-      </c>
-      <c r="K39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23">
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" s="5" t="s">
         <v>86</v>
       </c>
@@ -9144,14 +8867,8 @@
       <c r="I40" s="7">
         <v>41.3452214853301</v>
       </c>
-      <c r="J40" s="27">
-        <v>22.42</v>
-      </c>
-      <c r="K40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23">
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" s="5" t="s">
         <v>88</v>
       </c>
@@ -9179,14 +8896,8 @@
       <c r="I41" s="7">
         <v>41.588879874694399</v>
       </c>
-      <c r="J41" s="31">
-        <v>50.89</v>
-      </c>
-      <c r="K41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23">
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" s="5" t="s">
         <v>90</v>
       </c>
@@ -9214,17 +8925,11 @@
       <c r="I42" s="7">
         <v>42.3856958435208</v>
       </c>
-      <c r="J42" s="31">
-        <v>7.8</v>
-      </c>
-      <c r="K42" t="s">
-        <v>194</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:W37">
-    <sortCondition ref="Q3:Q37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:U37">
     <sortCondition ref="O3:O37"/>
+    <sortCondition ref="M3:M37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9234,8 +8939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9244,1047 +8949,1047 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="15">
+        <v>27.86</v>
+      </c>
+      <c r="F2" s="15">
+        <v>-175.85</v>
+      </c>
+      <c r="G2" s="15">
+        <v>467.27</v>
+      </c>
+      <c r="H2" s="15">
+        <v>5.73</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="27">
-        <v>27.86</v>
-      </c>
-      <c r="F2" s="27">
-        <v>-175.85</v>
-      </c>
-      <c r="G2" s="27">
-        <v>467.27</v>
-      </c>
-      <c r="H2" s="27">
-        <v>5.73</v>
-      </c>
-      <c r="I2" s="26" t="s">
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="28" t="s">
+      <c r="B3" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="C3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="19">
+        <v>25.41</v>
+      </c>
+      <c r="F3" s="19">
+        <v>-170.58</v>
+      </c>
+      <c r="G3" s="19">
+        <v>1075.44</v>
+      </c>
+      <c r="H3" s="19">
+        <v>3.03</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="B4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E4" s="19">
+        <v>23.79</v>
+      </c>
+      <c r="F4" s="19">
+        <v>-166.21</v>
+      </c>
+      <c r="G4" s="19">
+        <v>677.96</v>
+      </c>
+      <c r="H4" s="19">
+        <v>4.96</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="31">
-        <v>25.41</v>
-      </c>
-      <c r="F3" s="31">
-        <v>-170.58</v>
-      </c>
-      <c r="G3" s="31">
-        <v>1075.44</v>
-      </c>
-      <c r="H3" s="31">
-        <v>3.03</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="39">
-      <c r="A4" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="29" t="s">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="B5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="E5" s="19">
+        <v>26.01</v>
+      </c>
+      <c r="F5" s="19">
+        <v>-173.95</v>
+      </c>
+      <c r="G5" s="19">
+        <v>1004.27</v>
+      </c>
+      <c r="H5" s="19">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="31">
-        <v>23.79</v>
-      </c>
-      <c r="F4" s="31">
-        <v>-166.21</v>
-      </c>
-      <c r="G4" s="31">
-        <v>677.96</v>
-      </c>
-      <c r="H4" s="31">
-        <v>4.96</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="29" t="s">
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="B6" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="19">
+        <v>22.09</v>
+      </c>
+      <c r="F6" s="19">
+        <v>-159.57</v>
+      </c>
+      <c r="G6" s="19">
+        <v>241.7</v>
+      </c>
+      <c r="H6" s="19">
+        <v>6.22</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="19">
+        <v>23.58</v>
+      </c>
+      <c r="F7" s="19">
+        <v>-164.7</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1028.32</v>
+      </c>
+      <c r="H7" s="20">
+        <v>8.4</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="E8" s="19">
+        <v>28.42</v>
+      </c>
+      <c r="F8" s="19">
+        <v>-178.33</v>
+      </c>
+      <c r="G8" s="19">
+        <v>83.15</v>
+      </c>
+      <c r="H8" s="19">
+        <v>4.87</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="31">
-        <v>26.01</v>
-      </c>
-      <c r="F5" s="31">
-        <v>-173.95</v>
-      </c>
-      <c r="G5" s="31">
-        <v>1004.27</v>
-      </c>
-      <c r="H5" s="31">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="29" t="s">
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="D9" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="E9" s="19">
+        <v>21.49</v>
+      </c>
+      <c r="F9" s="19">
+        <v>-158</v>
+      </c>
+      <c r="G9" s="19">
+        <v>422.72</v>
+      </c>
+      <c r="H9" s="19">
+        <v>4.84</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="31">
-        <v>22.09</v>
-      </c>
-      <c r="F6" s="31">
-        <v>-159.57</v>
-      </c>
-      <c r="G6" s="31">
-        <v>241.7</v>
-      </c>
-      <c r="H6" s="31">
-        <v>6.22</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="30" t="s">
+    </row>
+    <row r="10" spans="1:9" ht="26">
+      <c r="A10" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="19">
+        <v>20.83</v>
+      </c>
+      <c r="F10" s="19">
+        <v>-156.75</v>
+      </c>
+      <c r="G10" s="19">
+        <v>450.84</v>
+      </c>
+      <c r="H10" s="19">
+        <v>2.68</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="E11" s="19">
+        <v>28.23</v>
+      </c>
+      <c r="F11" s="19">
+        <v>-177.38</v>
+      </c>
+      <c r="G11" s="19">
+        <v>101.52</v>
+      </c>
+      <c r="H11" s="20">
+        <v>4.7</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="19">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="F12" s="19">
+        <v>-169.52</v>
+      </c>
+      <c r="G12" s="19">
+        <v>194.01</v>
+      </c>
+      <c r="H12" s="19">
+        <v>23.73</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="19">
+        <v>-14.3</v>
+      </c>
+      <c r="F13" s="19">
+        <v>-170.7</v>
+      </c>
+      <c r="G13" s="19">
+        <v>50.89</v>
+      </c>
+      <c r="H13" s="19">
+        <v>6.39</v>
+      </c>
+      <c r="I13" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="31">
-        <v>23.58</v>
-      </c>
-      <c r="F7" s="31">
-        <v>-164.7</v>
-      </c>
-      <c r="G7" s="31">
-        <v>1028.32</v>
-      </c>
-      <c r="H7" s="32">
-        <v>8.4</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="30" t="s">
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="19">
+        <v>25.78</v>
+      </c>
+      <c r="F14" s="19">
+        <v>-171.73</v>
+      </c>
+      <c r="G14" s="19">
+        <v>488.13</v>
+      </c>
+      <c r="H14" s="19">
+        <v>10.36</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="E15" s="19">
+        <v>-14.55</v>
+      </c>
+      <c r="F15" s="19">
+        <v>-168.16</v>
+      </c>
+      <c r="G15" s="19">
+        <v>7.8</v>
+      </c>
+      <c r="H15" s="19">
+        <v>43.61</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="31">
-        <v>28.42</v>
-      </c>
-      <c r="F8" s="31">
-        <v>-178.33</v>
-      </c>
-      <c r="G8" s="31">
-        <v>83.15</v>
-      </c>
-      <c r="H8" s="31">
-        <v>4.87</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="30" t="s">
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="E16" s="19">
+        <v>19.53</v>
+      </c>
+      <c r="F16" s="19">
+        <v>-155.41999999999999</v>
+      </c>
+      <c r="G16" s="19">
+        <v>201.67</v>
+      </c>
+      <c r="H16" s="19">
+        <v>4.84</v>
+      </c>
+      <c r="I16" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="31">
-        <v>21.49</v>
-      </c>
-      <c r="F9" s="31">
-        <v>-158</v>
-      </c>
-      <c r="G9" s="31">
-        <v>422.72</v>
-      </c>
-      <c r="H9" s="31">
-        <v>4.84</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="65">
-      <c r="A10" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="30" t="s">
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="19">
+        <v>6.4</v>
+      </c>
+      <c r="F17" s="19">
+        <v>-162.38</v>
+      </c>
+      <c r="G17" s="19">
+        <v>47.63</v>
+      </c>
+      <c r="H17" s="19">
+        <v>23.88</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="E18" s="19">
+        <v>15.01</v>
+      </c>
+      <c r="F18" s="19">
+        <v>145.65</v>
+      </c>
+      <c r="G18" s="19">
+        <v>95.15</v>
+      </c>
+      <c r="H18" s="19">
+        <v>12.2</v>
+      </c>
+      <c r="I18" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E10" s="31">
-        <v>20.83</v>
-      </c>
-      <c r="F10" s="31">
-        <v>-156.75</v>
-      </c>
-      <c r="G10" s="31">
-        <v>450.84</v>
-      </c>
-      <c r="H10" s="31">
-        <v>2.68</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="30" t="s">
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="19">
+        <v>21.9</v>
+      </c>
+      <c r="F19" s="19">
+        <v>-160.15</v>
+      </c>
+      <c r="G19" s="19">
+        <v>108.06</v>
+      </c>
+      <c r="H19" s="19">
+        <v>5.27</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="E20" s="19">
+        <v>19.3</v>
+      </c>
+      <c r="F20" s="19">
+        <v>166.62</v>
+      </c>
+      <c r="G20" s="19">
+        <v>19.18</v>
+      </c>
+      <c r="H20" s="20">
+        <v>41.4</v>
+      </c>
+      <c r="I20" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="31">
-        <v>28.23</v>
-      </c>
-      <c r="F11" s="31">
-        <v>-177.38</v>
-      </c>
-      <c r="G11" s="31">
-        <v>101.52</v>
-      </c>
-      <c r="H11" s="32">
-        <v>4.7</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="29" t="s">
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="19">
+        <v>13.46</v>
+      </c>
+      <c r="F21" s="19">
+        <v>144.79</v>
+      </c>
+      <c r="G21" s="19">
+        <v>94.85</v>
+      </c>
+      <c r="H21" s="19">
+        <v>15.16</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="30" t="s">
+      <c r="D22" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="19">
+        <v>5.88</v>
+      </c>
+      <c r="F22" s="19">
+        <v>-162.09</v>
+      </c>
+      <c r="G22" s="19">
+        <v>52.5</v>
+      </c>
+      <c r="H22" s="19">
+        <v>31.91</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="31">
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="19">
+        <v>-176.48</v>
+      </c>
+      <c r="G23" s="19">
+        <v>4.43</v>
+      </c>
+      <c r="H23" s="19">
+        <v>26.24</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="19">
+        <v>20.55</v>
+      </c>
+      <c r="F24" s="19">
+        <v>144.88999999999999</v>
+      </c>
+      <c r="G24" s="19">
+        <v>1.38</v>
+      </c>
+      <c r="H24" s="19">
+        <v>24.98</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="19">
+        <v>18.11</v>
+      </c>
+      <c r="F25" s="19">
+        <v>145.76</v>
+      </c>
+      <c r="G25" s="19">
+        <v>16.29</v>
+      </c>
+      <c r="H25" s="19">
+        <v>19.89</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="19">
+        <v>20.02</v>
+      </c>
+      <c r="F26" s="19">
+        <v>145.22</v>
+      </c>
+      <c r="G26" s="19">
+        <v>3.17</v>
+      </c>
+      <c r="H26" s="19">
+        <v>27.28</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="19">
+        <v>-14.21</v>
+      </c>
+      <c r="F27" s="19">
+        <v>-169.56</v>
+      </c>
+      <c r="G27" s="19">
+        <v>22.42</v>
+      </c>
+      <c r="H27" s="19">
+        <v>20.53</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="19">
+        <v>-0.37</v>
+      </c>
+      <c r="F28" s="19">
+        <v>-160</v>
+      </c>
+      <c r="G28" s="19">
+        <v>4.32</v>
+      </c>
+      <c r="H28" s="22">
+        <v>29</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="19">
+        <v>-11.06</v>
+      </c>
+      <c r="F29" s="19">
+        <v>-171.08</v>
+      </c>
+      <c r="G29" s="19">
+        <v>2.82</v>
+      </c>
+      <c r="H29" s="19">
+        <v>51.41</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="19">
+        <v>-176.62</v>
+      </c>
+      <c r="G30" s="19">
+        <v>2.57</v>
+      </c>
+      <c r="H30" s="19">
+        <v>26.48</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="19">
+        <v>17.309999999999999</v>
+      </c>
+      <c r="F31" s="19">
+        <v>145.84</v>
+      </c>
+      <c r="G31" s="19">
+        <v>2</v>
+      </c>
+      <c r="H31" s="19">
+        <v>21.46</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="19">
+        <v>16.71</v>
+      </c>
+      <c r="F32" s="19">
+        <v>145.78</v>
+      </c>
+      <c r="G32" s="19">
+        <v>2</v>
+      </c>
+      <c r="H32" s="19">
         <v>16.739999999999998</v>
       </c>
-      <c r="F12" s="31">
-        <v>-169.52</v>
-      </c>
-      <c r="G12" s="31">
-        <v>194.01</v>
-      </c>
-      <c r="H12" s="31">
-        <v>23.73</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="30" t="s">
+      <c r="I32" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="19">
+        <v>19.690000000000001</v>
+      </c>
+      <c r="F33" s="19">
+        <v>145.4</v>
+      </c>
+      <c r="G33" s="19">
+        <v>2.54</v>
+      </c>
+      <c r="H33" s="19">
+        <v>16.32</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="19">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F34" s="19">
+        <v>145.83000000000001</v>
+      </c>
+      <c r="G34" s="19">
+        <v>4.28</v>
+      </c>
+      <c r="H34" s="19">
+        <v>23.65</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="19">
+        <v>14.16</v>
+      </c>
+      <c r="F35" s="19">
+        <v>145.21</v>
+      </c>
+      <c r="G35" s="19">
+        <v>16.03</v>
+      </c>
+      <c r="H35" s="19">
+        <v>12.34</v>
+      </c>
+      <c r="I35" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E13" s="31">
-        <v>-14.3</v>
-      </c>
-      <c r="F13" s="31">
-        <v>-170.7</v>
-      </c>
-      <c r="G13" s="31">
-        <v>50.89</v>
-      </c>
-      <c r="H13" s="31">
-        <v>6.39</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="31">
-        <v>25.78</v>
-      </c>
-      <c r="F14" s="31">
-        <v>-171.73</v>
-      </c>
-      <c r="G14" s="31">
-        <v>488.13</v>
-      </c>
-      <c r="H14" s="31">
-        <v>10.36</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="30" t="s">
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="25">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="F36" s="25">
+        <v>145.66</v>
+      </c>
+      <c r="G36" s="25">
+        <v>9.5</v>
+      </c>
+      <c r="H36" s="25">
+        <v>23.03</v>
+      </c>
+      <c r="I36" s="24" t="s">
         <v>116</v>
-      </c>
-      <c r="E15" s="31">
-        <v>-14.55</v>
-      </c>
-      <c r="F15" s="31">
-        <v>-168.16</v>
-      </c>
-      <c r="G15" s="31">
-        <v>7.8</v>
-      </c>
-      <c r="H15" s="31">
-        <v>43.61</v>
-      </c>
-      <c r="I15" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E16" s="31">
-        <v>19.53</v>
-      </c>
-      <c r="F16" s="31">
-        <v>-155.41999999999999</v>
-      </c>
-      <c r="G16" s="31">
-        <v>201.67</v>
-      </c>
-      <c r="H16" s="31">
-        <v>4.84</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" s="31">
-        <v>6.4</v>
-      </c>
-      <c r="F17" s="31">
-        <v>-162.38</v>
-      </c>
-      <c r="G17" s="31">
-        <v>47.63</v>
-      </c>
-      <c r="H17" s="31">
-        <v>23.88</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="39">
-      <c r="A18" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E18" s="31">
-        <v>15.01</v>
-      </c>
-      <c r="F18" s="31">
-        <v>145.65</v>
-      </c>
-      <c r="G18" s="31">
-        <v>95.15</v>
-      </c>
-      <c r="H18" s="31">
-        <v>12.2</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="31">
-        <v>21.9</v>
-      </c>
-      <c r="F19" s="31">
-        <v>-160.15</v>
-      </c>
-      <c r="G19" s="31">
-        <v>108.06</v>
-      </c>
-      <c r="H19" s="31">
-        <v>5.27</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" s="31">
-        <v>19.3</v>
-      </c>
-      <c r="F20" s="31">
-        <v>166.62</v>
-      </c>
-      <c r="G20" s="31">
-        <v>19.18</v>
-      </c>
-      <c r="H20" s="32">
-        <v>41.4</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E21" s="31">
-        <v>13.46</v>
-      </c>
-      <c r="F21" s="31">
-        <v>144.79</v>
-      </c>
-      <c r="G21" s="31">
-        <v>94.85</v>
-      </c>
-      <c r="H21" s="31">
-        <v>15.16</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="31">
-        <v>5.88</v>
-      </c>
-      <c r="F22" s="31">
-        <v>-162.09</v>
-      </c>
-      <c r="G22" s="31">
-        <v>52.5</v>
-      </c>
-      <c r="H22" s="31">
-        <v>31.91</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="31">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="31">
-        <v>-176.48</v>
-      </c>
-      <c r="G23" s="31">
-        <v>4.43</v>
-      </c>
-      <c r="H23" s="31">
-        <v>26.24</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="26">
-      <c r="A24" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="31">
-        <v>20.55</v>
-      </c>
-      <c r="F24" s="31">
-        <v>144.88999999999999</v>
-      </c>
-      <c r="G24" s="31">
-        <v>1.38</v>
-      </c>
-      <c r="H24" s="31">
-        <v>24.98</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="31">
-        <v>18.11</v>
-      </c>
-      <c r="F25" s="31">
-        <v>145.76</v>
-      </c>
-      <c r="G25" s="31">
-        <v>16.29</v>
-      </c>
-      <c r="H25" s="31">
-        <v>19.89</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E26" s="31">
-        <v>20.02</v>
-      </c>
-      <c r="F26" s="31">
-        <v>145.22</v>
-      </c>
-      <c r="G26" s="31">
-        <v>3.17</v>
-      </c>
-      <c r="H26" s="31">
-        <v>27.28</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="39">
-      <c r="A27" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="31">
-        <v>-14.21</v>
-      </c>
-      <c r="F27" s="31">
-        <v>-169.56</v>
-      </c>
-      <c r="G27" s="31">
-        <v>22.42</v>
-      </c>
-      <c r="H27" s="31">
-        <v>20.53</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="31">
-        <v>-0.37</v>
-      </c>
-      <c r="F28" s="31">
-        <v>-160</v>
-      </c>
-      <c r="G28" s="31">
-        <v>4.32</v>
-      </c>
-      <c r="H28" s="34">
-        <v>29</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="31">
-        <v>-11.06</v>
-      </c>
-      <c r="F29" s="31">
-        <v>-171.08</v>
-      </c>
-      <c r="G29" s="31">
-        <v>2.82</v>
-      </c>
-      <c r="H29" s="31">
-        <v>51.41</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="31">
-        <v>0.8</v>
-      </c>
-      <c r="F30" s="31">
-        <v>-176.62</v>
-      </c>
-      <c r="G30" s="31">
-        <v>2.57</v>
-      </c>
-      <c r="H30" s="31">
-        <v>26.48</v>
-      </c>
-      <c r="I30" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="31">
-        <v>17.309999999999999</v>
-      </c>
-      <c r="F31" s="31">
-        <v>145.84</v>
-      </c>
-      <c r="G31" s="31">
-        <v>2</v>
-      </c>
-      <c r="H31" s="31">
-        <v>21.46</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="31">
-        <v>16.71</v>
-      </c>
-      <c r="F32" s="31">
-        <v>145.78</v>
-      </c>
-      <c r="G32" s="31">
-        <v>2</v>
-      </c>
-      <c r="H32" s="31">
-        <v>16.739999999999998</v>
-      </c>
-      <c r="I32" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="31">
-        <v>19.690000000000001</v>
-      </c>
-      <c r="F33" s="31">
-        <v>145.4</v>
-      </c>
-      <c r="G33" s="31">
-        <v>2.54</v>
-      </c>
-      <c r="H33" s="31">
-        <v>16.32</v>
-      </c>
-      <c r="I33" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="31">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="F34" s="31">
-        <v>145.83000000000001</v>
-      </c>
-      <c r="G34" s="31">
-        <v>4.28</v>
-      </c>
-      <c r="H34" s="31">
-        <v>23.65</v>
-      </c>
-      <c r="I34" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E35" s="31">
-        <v>14.16</v>
-      </c>
-      <c r="F35" s="31">
-        <v>145.21</v>
-      </c>
-      <c r="G35" s="31">
-        <v>16.03</v>
-      </c>
-      <c r="H35" s="31">
-        <v>12.34</v>
-      </c>
-      <c r="I35" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="D36" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="37">
-        <v>18.760000000000002</v>
-      </c>
-      <c r="F36" s="37">
-        <v>145.66</v>
-      </c>
-      <c r="G36" s="37">
-        <v>9.5</v>
-      </c>
-      <c r="H36" s="37">
-        <v>23.03</v>
-      </c>
-      <c r="I36" s="36" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ime crep covariates to be island complex means
</commit_message>
<xml_diff>
--- a/data/crep_oceanographic/Gove2013_pone.0061974.s005.xlsx
+++ b/data/crep_oceanographic/Gove2013_pone.0061974.s005.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrobinson/Documents/git-repos/PelagicReefs/data/crep_oceanographic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robins64/Documents/git_repos/PelagicReefs/data/crep_oceanographic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755AFBD5-8771-EE43-BB37-8087C6AC5801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035ACA79-E323-DD4E-9051-88DD7AFE0BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Gove2014_SuppTable2" sheetId="3" r:id="rId3"/>
+    <sheet name="Gove2013_TableS1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gove2013_condensed" sheetId="2" r:id="rId2"/>
+    <sheet name="Gove 2013 Table 1" sheetId="4" r:id="rId3"/>
+    <sheet name="Gove2016_SuppTable2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="201">
   <si>
     <t>Sea Surface Temperature (°C)</t>
   </si>
@@ -1339,6 +1340,36 @@
       <t>AGR</t>
     </r>
   </si>
+  <si>
+    <t>Island Name</t>
+  </si>
+  <si>
+    <t>Island Type</t>
+  </si>
+  <si>
+    <t>Land Area</t>
+  </si>
+  <si>
+    <t>Reef Area</t>
+  </si>
+  <si>
+    <t>Closed atoll</t>
+  </si>
+  <si>
+    <t>Pearl &amp; Hermes Reef</t>
+  </si>
+  <si>
+    <t>Open atoll</t>
+  </si>
+  <si>
+    <t>Carbonate island</t>
+  </si>
+  <si>
+    <t>Basalt island</t>
+  </si>
+  <si>
+    <t>Basalt/Carbonate island</t>
+  </si>
 </sst>
 </file>
 
@@ -1349,7 +1380,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1457,8 +1488,19 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1490,8 +1532,13 @@
         <fgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCDDDE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1593,6 +1640,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF231F20"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF231F20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF231F20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF231F20"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF231F20"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF231F20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF231F20"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF231F20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF231F20"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1606,7 +1706,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
@@ -1720,6 +1820,72 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2037,7 +2203,7 @@
   <dimension ref="A1:AO43"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:AO43"/>
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8936,11 +9102,1044 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00165DE3-66EA-BB41-A9F2-F3EAAFAE7FD1}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="40" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="40" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="40" customWidth="1"/>
+    <col min="5" max="6" width="10.5" style="40" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="40" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="40" customWidth="1"/>
+    <col min="9" max="16384" width="7.5" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="50">
+        <v>28.42</v>
+      </c>
+      <c r="E2" s="51">
+        <v>-178.33</v>
+      </c>
+      <c r="F2" s="51">
+        <v>0.92</v>
+      </c>
+      <c r="G2" s="51">
+        <v>83.15</v>
+      </c>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="55">
+        <v>28.23</v>
+      </c>
+      <c r="E3" s="56">
+        <v>-177.38</v>
+      </c>
+      <c r="F3" s="56">
+        <v>5.98</v>
+      </c>
+      <c r="G3" s="56">
+        <v>101.52</v>
+      </c>
+      <c r="H3" s="42"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="50">
+        <v>27.86</v>
+      </c>
+      <c r="E4" s="51">
+        <v>-175.85</v>
+      </c>
+      <c r="F4" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="51">
+        <v>467.27</v>
+      </c>
+      <c r="H4" s="42"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="55">
+        <v>26.01</v>
+      </c>
+      <c r="E5" s="56">
+        <v>-173.95</v>
+      </c>
+      <c r="F5" s="56">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="56">
+        <v>1004.27</v>
+      </c>
+      <c r="H5" s="42"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="50">
+        <v>25.78</v>
+      </c>
+      <c r="E6" s="51">
+        <v>-171.73</v>
+      </c>
+      <c r="F6" s="51">
+        <v>3.53</v>
+      </c>
+      <c r="G6" s="51">
+        <v>488.13</v>
+      </c>
+      <c r="H6" s="42"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="55">
+        <v>25.41</v>
+      </c>
+      <c r="E7" s="56">
+        <v>-170.58</v>
+      </c>
+      <c r="F7" s="56">
+        <v>0</v>
+      </c>
+      <c r="G7" s="56">
+        <v>1075.44</v>
+      </c>
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="50">
+        <v>23.79</v>
+      </c>
+      <c r="E8" s="51">
+        <v>-166.21</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="51">
+        <v>677.96</v>
+      </c>
+      <c r="H8" s="42"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="55">
+        <v>23.58</v>
+      </c>
+      <c r="E9" s="56">
+        <v>-164.7</v>
+      </c>
+      <c r="F9" s="56">
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="56">
+        <v>1028.32</v>
+      </c>
+      <c r="H9" s="42"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="50">
+        <v>23.06</v>
+      </c>
+      <c r="E10" s="51">
+        <v>-161.93</v>
+      </c>
+      <c r="F10" s="51">
+        <v>0.72</v>
+      </c>
+      <c r="G10" s="51">
+        <v>0.74</v>
+      </c>
+      <c r="H10" s="42"/>
+    </row>
+    <row r="11" spans="1:8" ht="30">
+      <c r="A11" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="50">
+        <v>22.09</v>
+      </c>
+      <c r="E11" s="51">
+        <v>-159.57</v>
+      </c>
+      <c r="F11" s="51">
+        <v>1436.7</v>
+      </c>
+      <c r="G11" s="51">
+        <v>241.7</v>
+      </c>
+      <c r="H11" s="42"/>
+    </row>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" s="55">
+        <v>21.9</v>
+      </c>
+      <c r="E12" s="56">
+        <v>-160.15</v>
+      </c>
+      <c r="F12" s="56">
+        <v>186.82</v>
+      </c>
+      <c r="G12" s="56">
+        <v>108.06</v>
+      </c>
+      <c r="H12" s="42"/>
+    </row>
+    <row r="13" spans="1:8" ht="30">
+      <c r="A13" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="50">
+        <v>21.49</v>
+      </c>
+      <c r="E13" s="51">
+        <v>-158</v>
+      </c>
+      <c r="F13" s="51">
+        <v>1548.99</v>
+      </c>
+      <c r="G13" s="51">
+        <v>422.72</v>
+      </c>
+      <c r="H13" s="42"/>
+    </row>
+    <row r="14" spans="1:8" ht="30">
+      <c r="A14" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="55">
+        <v>21.14</v>
+      </c>
+      <c r="E14" s="56">
+        <v>-157.09</v>
+      </c>
+      <c r="F14" s="56">
+        <v>670.22</v>
+      </c>
+      <c r="G14" s="56">
+        <v>198.51</v>
+      </c>
+      <c r="H14" s="42"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="50">
+        <v>20.82</v>
+      </c>
+      <c r="E15" s="51">
+        <v>-156.91999999999999</v>
+      </c>
+      <c r="F15" s="51">
+        <v>365.37</v>
+      </c>
+      <c r="G15" s="51">
+        <v>55.49</v>
+      </c>
+      <c r="H15" s="42"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="55">
+        <v>20.82</v>
+      </c>
+      <c r="E16" s="56">
+        <v>-156.4</v>
+      </c>
+      <c r="F16" s="56">
+        <v>1886.32</v>
+      </c>
+      <c r="G16" s="56">
+        <v>196.84</v>
+      </c>
+      <c r="H16" s="42"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="50">
+        <v>19.53</v>
+      </c>
+      <c r="E17" s="51">
+        <v>-155.41999999999999</v>
+      </c>
+      <c r="F17" s="51">
+        <v>10441.51</v>
+      </c>
+      <c r="G17" s="51">
+        <v>201.67</v>
+      </c>
+      <c r="H17" s="42"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="55">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="E18" s="56">
+        <v>-169.52</v>
+      </c>
+      <c r="F18" s="56">
+        <v>2.63</v>
+      </c>
+      <c r="G18" s="56">
+        <v>194.01</v>
+      </c>
+      <c r="H18" s="42"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="55">
+        <v>19.3</v>
+      </c>
+      <c r="E19" s="56">
+        <v>166.62</v>
+      </c>
+      <c r="F19" s="56">
+        <v>6.97</v>
+      </c>
+      <c r="G19" s="56">
+        <v>19.18</v>
+      </c>
+      <c r="H19" s="42"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="50">
+        <v>20.55</v>
+      </c>
+      <c r="E20" s="51">
+        <v>144.88999999999999</v>
+      </c>
+      <c r="F20" s="51">
+        <v>2.25</v>
+      </c>
+      <c r="G20" s="51">
+        <v>1.38</v>
+      </c>
+      <c r="H20" s="42"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="55">
+        <v>20.02</v>
+      </c>
+      <c r="E21" s="56">
+        <v>145.22</v>
+      </c>
+      <c r="F21" s="56">
+        <v>2.14</v>
+      </c>
+      <c r="G21" s="56">
+        <v>3.17</v>
+      </c>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="50">
+        <v>19.690000000000001</v>
+      </c>
+      <c r="E22" s="51">
+        <v>145.4</v>
+      </c>
+      <c r="F22" s="51">
+        <v>7.86</v>
+      </c>
+      <c r="G22" s="51">
+        <v>2.54</v>
+      </c>
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="55">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="E23" s="56">
+        <v>145.66</v>
+      </c>
+      <c r="F23" s="56">
+        <v>44.05</v>
+      </c>
+      <c r="G23" s="56">
+        <v>9.5</v>
+      </c>
+      <c r="H23" s="42"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="50">
+        <v>18.11</v>
+      </c>
+      <c r="E24" s="51">
+        <v>145.76</v>
+      </c>
+      <c r="F24" s="51">
+        <v>47.75</v>
+      </c>
+      <c r="G24" s="51">
+        <v>16.29</v>
+      </c>
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="55">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E25" s="56">
+        <v>145.83000000000001</v>
+      </c>
+      <c r="F25" s="56">
+        <v>12.96</v>
+      </c>
+      <c r="G25" s="56">
+        <v>4.28</v>
+      </c>
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="50">
+        <v>17.309999999999999</v>
+      </c>
+      <c r="E26" s="51">
+        <v>145.84</v>
+      </c>
+      <c r="F26" s="51">
+        <v>4.24</v>
+      </c>
+      <c r="G26" s="51">
+        <v>2</v>
+      </c>
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="55">
+        <v>16.71</v>
+      </c>
+      <c r="E27" s="56">
+        <v>145.78</v>
+      </c>
+      <c r="F27" s="56">
+        <v>4.47</v>
+      </c>
+      <c r="G27" s="56">
+        <v>2</v>
+      </c>
+      <c r="H27" s="42"/>
+    </row>
+    <row r="28" spans="1:8" ht="30">
+      <c r="A28" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="50">
+        <v>15.19</v>
+      </c>
+      <c r="E28" s="51">
+        <v>145.75</v>
+      </c>
+      <c r="F28" s="51">
+        <v>118.98</v>
+      </c>
+      <c r="G28" s="51">
+        <v>73.040000000000006</v>
+      </c>
+      <c r="H28" s="42"/>
+    </row>
+    <row r="29" spans="1:8" ht="30">
+      <c r="A29" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D29" s="55">
+        <v>14.99</v>
+      </c>
+      <c r="E29" s="56">
+        <v>145.63</v>
+      </c>
+      <c r="F29" s="56">
+        <v>101.21</v>
+      </c>
+      <c r="G29" s="56">
+        <v>16.2</v>
+      </c>
+      <c r="H29" s="42"/>
+    </row>
+    <row r="30" spans="1:8" ht="30">
+      <c r="A30" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30" s="50">
+        <v>14.85</v>
+      </c>
+      <c r="E30" s="51">
+        <v>145.55000000000001</v>
+      </c>
+      <c r="F30" s="51">
+        <v>7.01</v>
+      </c>
+      <c r="G30" s="51">
+        <v>5.91</v>
+      </c>
+      <c r="H30" s="42"/>
+    </row>
+    <row r="31" spans="1:8" ht="30">
+      <c r="A31" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D31" s="55">
+        <v>14.16</v>
+      </c>
+      <c r="E31" s="56">
+        <v>145.21</v>
+      </c>
+      <c r="F31" s="56">
+        <v>85.13</v>
+      </c>
+      <c r="G31" s="56">
+        <v>16.03</v>
+      </c>
+      <c r="H31" s="42"/>
+    </row>
+    <row r="32" spans="1:8" ht="30">
+      <c r="A32" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32" s="50">
+        <v>13.46</v>
+      </c>
+      <c r="E32" s="51">
+        <v>144.79</v>
+      </c>
+      <c r="F32" s="51">
+        <v>544.34</v>
+      </c>
+      <c r="G32" s="51">
+        <v>94.85</v>
+      </c>
+      <c r="H32" s="42"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="50">
+        <v>6.4</v>
+      </c>
+      <c r="E33" s="51">
+        <v>-162.38</v>
+      </c>
+      <c r="F33" s="51">
+        <v>0.76</v>
+      </c>
+      <c r="G33" s="51">
+        <v>47.63</v>
+      </c>
+      <c r="H33" s="42"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="D34" s="55">
+        <v>5.88</v>
+      </c>
+      <c r="E34" s="56">
+        <v>-162.09</v>
+      </c>
+      <c r="F34" s="56">
+        <v>2.23</v>
+      </c>
+      <c r="G34" s="56">
+        <v>52.5</v>
+      </c>
+      <c r="H34" s="42"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="E35" s="51">
+        <v>-176.62</v>
+      </c>
+      <c r="F35" s="51">
+        <v>1.8</v>
+      </c>
+      <c r="G35" s="51">
+        <v>2.57</v>
+      </c>
+      <c r="H35" s="42"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="E36" s="56">
+        <v>-176.48</v>
+      </c>
+      <c r="F36" s="56">
+        <v>1.6</v>
+      </c>
+      <c r="G36" s="56">
+        <v>4.43</v>
+      </c>
+      <c r="H36" s="42"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="50">
+        <v>20.37</v>
+      </c>
+      <c r="E37" s="51">
+        <v>-160</v>
+      </c>
+      <c r="F37" s="51">
+        <v>4.43</v>
+      </c>
+      <c r="G37" s="51">
+        <v>4.32</v>
+      </c>
+      <c r="H37" s="42"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="D38" s="50">
+        <v>211.06</v>
+      </c>
+      <c r="E38" s="51">
+        <v>-171.08</v>
+      </c>
+      <c r="F38" s="51">
+        <v>2.38</v>
+      </c>
+      <c r="G38" s="51">
+        <v>2.82</v>
+      </c>
+      <c r="H38" s="42"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" s="55">
+        <v>214.17</v>
+      </c>
+      <c r="E39" s="56">
+        <v>-169.65</v>
+      </c>
+      <c r="F39" s="56">
+        <v>12.61</v>
+      </c>
+      <c r="G39" s="56">
+        <v>12.03</v>
+      </c>
+      <c r="H39" s="42"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" s="50">
+        <v>214.24</v>
+      </c>
+      <c r="E40" s="51">
+        <v>-169.47</v>
+      </c>
+      <c r="F40" s="51">
+        <v>45.09</v>
+      </c>
+      <c r="G40" s="51">
+        <v>10.38</v>
+      </c>
+      <c r="H40" s="42"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" s="55">
+        <v>214.3</v>
+      </c>
+      <c r="E41" s="56">
+        <v>-170.7</v>
+      </c>
+      <c r="F41" s="56">
+        <v>137.44999999999999</v>
+      </c>
+      <c r="G41" s="56">
+        <v>50.89</v>
+      </c>
+      <c r="H41" s="42"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="D42" s="60">
+        <v>214.55</v>
+      </c>
+      <c r="E42" s="61">
+        <v>-168.16</v>
+      </c>
+      <c r="F42" s="61">
+        <v>0.09</v>
+      </c>
+      <c r="G42" s="61">
+        <v>7.8</v>
+      </c>
+      <c r="H42" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>